<commit_message>
Terminando la segunda bitacora
</commit_message>
<xml_diff>
--- a/BitacoraDos.xlsx
+++ b/BitacoraDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Jhon\Bitacoras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FB7165-5696-4FBE-9D18-83875FAB6DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0745D307-EEF2-43FD-AA79-AED416E55CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -994,61 +994,40 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1060,44 +1039,59 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1118,34 +1112,63 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1167,29 +1190,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1628,47 +1628,47 @@
   <sheetData>
     <row r="1" spans="2:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="46"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="37"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="36"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="2:15" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="41"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="39"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="2:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="37"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="36"/>
       <c r="K4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1677,15 +1677,15 @@
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="41"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="43"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="39"/>
       <c r="K5" s="3" t="s">
         <v>2</v>
       </c>
@@ -1695,7 +1695,7 @@
       <c r="O5" s="1"/>
     </row>
     <row r="6" spans="2:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="41" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="31"/>
@@ -1709,7 +1709,7 @@
       <c r="K6" s="32"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="41" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="31"/>
@@ -1723,7 +1723,7 @@
       <c r="K7" s="32"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="42" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="31"/>
@@ -1737,165 +1737,165 @@
       <c r="K8" s="32"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="37"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="36"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="40"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="46"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="38"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="40"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="46"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="38"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="40"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="46"/>
     </row>
     <row r="13" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="38"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="40"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="45"/>
+      <c r="K13" s="46"/>
     </row>
     <row r="14" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="38"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="40"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="46"/>
     </row>
     <row r="15" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="38"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="40"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="46"/>
     </row>
     <row r="16" spans="2:15" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="40"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="46"/>
     </row>
     <row r="17" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="38"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="40"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="46"/>
     </row>
     <row r="18" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="38"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="40"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="46"/>
     </row>
     <row r="19" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="38"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="40"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="46"/>
     </row>
     <row r="20" spans="2:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="38"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="40"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
+      <c r="K20" s="46"/>
     </row>
     <row r="21" spans="2:12" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="41"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="43"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="39"/>
     </row>
     <row r="22" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="44" t="s">
+      <c r="B22" s="42" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="31"/>
@@ -1909,7 +1909,7 @@
       <c r="K22" s="32"/>
     </row>
     <row r="23" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="44"/>
+      <c r="B23" s="42"/>
       <c r="C23" s="31"/>
       <c r="D23" s="31"/>
       <c r="E23" s="31"/>
@@ -1924,14 +1924,14 @@
       <c r="B24" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="45" t="s">
+      <c r="C24" s="47" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="31"/>
       <c r="E24" s="31"/>
       <c r="F24" s="31"/>
       <c r="G24" s="32"/>
-      <c r="H24" s="45" t="s">
+      <c r="H24" s="47" t="s">
         <v>10</v>
       </c>
       <c r="I24" s="31"/>
@@ -1951,9 +1951,9 @@
       <c r="F25" s="31"/>
       <c r="G25" s="32"/>
       <c r="H25" s="30"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="33"/>
-      <c r="K25" s="34"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="49"/>
     </row>
     <row r="26" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
@@ -1983,9 +1983,9 @@
       <c r="F27" s="31"/>
       <c r="G27" s="32"/>
       <c r="H27" s="30"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="34"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="49"/>
     </row>
     <row r="28" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
@@ -2017,9 +2017,9 @@
       <c r="H29" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="34"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="48"/>
+      <c r="K29" s="49"/>
     </row>
     <row r="30" spans="2:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
@@ -2035,9 +2035,9 @@
       <c r="H30" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="34"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="49"/>
     </row>
     <row r="31" spans="2:12" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
@@ -2053,9 +2053,9 @@
       <c r="H31" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="34"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="49"/>
     </row>
     <row r="32" spans="2:12" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
@@ -2069,9 +2069,9 @@
       <c r="F32" s="31"/>
       <c r="G32" s="32"/>
       <c r="H32" s="30"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="33"/>
-      <c r="K32" s="34"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="48"/>
+      <c r="K32" s="49"/>
     </row>
     <row r="33" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
@@ -2350,7 +2350,7 @@
       <c r="K49" s="32"/>
     </row>
     <row r="50" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="49"/>
+      <c r="B50" s="33"/>
       <c r="C50" s="31"/>
       <c r="D50" s="31"/>
       <c r="E50" s="31"/>
@@ -3335,6 +3335,55 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="60">
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="H43:K43"/>
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="H40:K40"/>
+    <mergeCell ref="H41:K41"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="H38:K38"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="H31:K31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="B9:K21"/>
+    <mergeCell ref="B22:K22"/>
+    <mergeCell ref="B23:K23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="H24:K24"/>
+    <mergeCell ref="B2:K3"/>
+    <mergeCell ref="B4:J5"/>
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="B8:K8"/>
     <mergeCell ref="C48:G48"/>
     <mergeCell ref="C49:G49"/>
     <mergeCell ref="H49:K49"/>
@@ -3346,55 +3395,6 @@
     <mergeCell ref="C47:G47"/>
     <mergeCell ref="H47:K47"/>
     <mergeCell ref="H48:K48"/>
-    <mergeCell ref="B2:K3"/>
-    <mergeCell ref="B4:J5"/>
-    <mergeCell ref="B6:K6"/>
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="B8:K8"/>
-    <mergeCell ref="B9:K21"/>
-    <mergeCell ref="B22:K22"/>
-    <mergeCell ref="B23:K23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="H24:K24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="H31:K31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="H38:K38"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="H39:K39"/>
-    <mergeCell ref="C43:G43"/>
-    <mergeCell ref="H43:K43"/>
-    <mergeCell ref="C44:G44"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="H40:K40"/>
-    <mergeCell ref="H41:K41"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="H42:K42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -3406,8 +3406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z7" sqref="Z7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AG26" sqref="AG26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3433,28 +3433,28 @@
   <sheetData>
     <row r="1" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13"/>
-      <c r="B1" s="74"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="40"/>
-      <c r="W1" s="75" t="s">
+      <c r="B1" s="72"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="73" t="s">
         <v>1</v>
       </c>
       <c r="X1" s="31"/>
@@ -3463,28 +3463,28 @@
     </row>
     <row r="2" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="76" t="s">
+      <c r="B2" s="44"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="45"/>
+      <c r="S2" s="45"/>
+      <c r="T2" s="45"/>
+      <c r="U2" s="45"/>
+      <c r="V2" s="46"/>
+      <c r="W2" s="74" t="s">
         <v>2</v>
       </c>
       <c r="X2" s="31"/>
@@ -3493,127 +3493,127 @@
     </row>
     <row r="3" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="75" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78"/>
-      <c r="N3" s="78"/>
-      <c r="O3" s="78"/>
-      <c r="P3" s="78"/>
-      <c r="Q3" s="78"/>
-      <c r="R3" s="78"/>
-      <c r="S3" s="78"/>
-      <c r="T3" s="78"/>
-      <c r="U3" s="78"/>
-      <c r="V3" s="78"/>
-      <c r="W3" s="78"/>
-      <c r="X3" s="78"/>
-      <c r="Y3" s="79"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="76"/>
+      <c r="N3" s="76"/>
+      <c r="O3" s="76"/>
+      <c r="P3" s="76"/>
+      <c r="Q3" s="76"/>
+      <c r="R3" s="76"/>
+      <c r="S3" s="76"/>
+      <c r="T3" s="76"/>
+      <c r="U3" s="76"/>
+      <c r="V3" s="76"/>
+      <c r="W3" s="76"/>
+      <c r="X3" s="76"/>
+      <c r="Y3" s="77"/>
       <c r="Z3" s="13"/>
     </row>
     <row r="4" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="75" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="78"/>
-      <c r="P4" s="78"/>
-      <c r="Q4" s="78"/>
-      <c r="R4" s="78"/>
-      <c r="S4" s="78"/>
-      <c r="T4" s="78"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="78"/>
-      <c r="W4" s="78"/>
-      <c r="X4" s="78"/>
-      <c r="Y4" s="79"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="76"/>
+      <c r="M4" s="76"/>
+      <c r="N4" s="76"/>
+      <c r="O4" s="76"/>
+      <c r="P4" s="76"/>
+      <c r="Q4" s="76"/>
+      <c r="R4" s="76"/>
+      <c r="S4" s="76"/>
+      <c r="T4" s="76"/>
+      <c r="U4" s="76"/>
+      <c r="V4" s="76"/>
+      <c r="W4" s="76"/>
+      <c r="X4" s="76"/>
+      <c r="Y4" s="77"/>
       <c r="Z4" s="13"/>
     </row>
     <row r="5" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="81"/>
-      <c r="L5" s="81"/>
-      <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="81"/>
-      <c r="Q5" s="81"/>
-      <c r="R5" s="81"/>
-      <c r="S5" s="81"/>
-      <c r="T5" s="81"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="81"/>
-      <c r="W5" s="81"/>
-      <c r="X5" s="81"/>
-      <c r="Y5" s="82"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="79"/>
+      <c r="Q5" s="79"/>
+      <c r="R5" s="79"/>
+      <c r="S5" s="79"/>
+      <c r="T5" s="79"/>
+      <c r="U5" s="79"/>
+      <c r="V5" s="79"/>
+      <c r="W5" s="79"/>
+      <c r="X5" s="79"/>
+      <c r="Y5" s="80"/>
       <c r="Z5" s="13"/>
     </row>
     <row r="6" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
-      <c r="B6" s="80" t="s">
+      <c r="B6" s="78" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="81"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="81"/>
-      <c r="H6" s="81"/>
-      <c r="I6" s="81"/>
-      <c r="J6" s="81"/>
-      <c r="K6" s="81"/>
-      <c r="L6" s="81"/>
-      <c r="M6" s="81"/>
-      <c r="N6" s="81"/>
-      <c r="O6" s="81"/>
-      <c r="P6" s="81"/>
-      <c r="Q6" s="81"/>
-      <c r="R6" s="81"/>
-      <c r="S6" s="81"/>
-      <c r="T6" s="81"/>
-      <c r="U6" s="81"/>
-      <c r="V6" s="81"/>
-      <c r="W6" s="81"/>
-      <c r="X6" s="81"/>
-      <c r="Y6" s="82"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="79"/>
+      <c r="G6" s="79"/>
+      <c r="H6" s="79"/>
+      <c r="I6" s="79"/>
+      <c r="J6" s="79"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="79"/>
+      <c r="N6" s="79"/>
+      <c r="O6" s="79"/>
+      <c r="P6" s="79"/>
+      <c r="Q6" s="79"/>
+      <c r="R6" s="79"/>
+      <c r="S6" s="79"/>
+      <c r="T6" s="79"/>
+      <c r="U6" s="79"/>
+      <c r="V6" s="79"/>
+      <c r="W6" s="79"/>
+      <c r="X6" s="79"/>
+      <c r="Y6" s="80"/>
       <c r="Z6" s="13"/>
     </row>
     <row r="7" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
-      <c r="B7" s="60" t="s">
+      <c r="B7" s="53" t="s">
         <v>64</v>
       </c>
       <c r="C7" s="31"/>
@@ -3643,35 +3643,35 @@
     </row>
     <row r="8" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
-      <c r="B8" s="83"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="36"/>
-      <c r="P8" s="36"/>
-      <c r="Q8" s="36"/>
-      <c r="R8" s="36"/>
-      <c r="S8" s="36"/>
-      <c r="T8" s="36"/>
-      <c r="U8" s="36"/>
-      <c r="V8" s="36"/>
-      <c r="W8" s="36"/>
-      <c r="X8" s="36"/>
-      <c r="Y8" s="36"/>
+      <c r="B8" s="66"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="35"/>
+      <c r="R8" s="35"/>
+      <c r="S8" s="35"/>
+      <c r="T8" s="35"/>
+      <c r="U8" s="35"/>
+      <c r="V8" s="35"/>
+      <c r="W8" s="35"/>
+      <c r="X8" s="35"/>
+      <c r="Y8" s="35"/>
       <c r="Z8" s="13"/>
     </row>
     <row r="9" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="57" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="31"/>
@@ -3684,18 +3684,18 @@
       <c r="J9" s="31"/>
       <c r="K9" s="31"/>
       <c r="L9" s="32"/>
-      <c r="M9" s="68" t="s">
+      <c r="M9" s="57" t="s">
         <v>65</v>
       </c>
       <c r="N9" s="31"/>
       <c r="O9" s="32"/>
-      <c r="P9" s="68" t="s">
+      <c r="P9" s="57" t="s">
         <v>66</v>
       </c>
       <c r="Q9" s="31"/>
       <c r="R9" s="31"/>
       <c r="S9" s="32"/>
-      <c r="T9" s="68" t="s">
+      <c r="T9" s="57" t="s">
         <v>17</v>
       </c>
       <c r="U9" s="31"/>
@@ -3707,38 +3707,38 @@
     </row>
     <row r="10" spans="1:26" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="81" t="s">
         <v>113</v>
       </c>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="61"/>
-      <c r="K10" s="61"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="54">
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="81">
         <v>900199836</v>
       </c>
       <c r="N10" s="31"/>
       <c r="O10" s="32"/>
-      <c r="P10" s="54">
+      <c r="P10" s="81">
         <v>2</v>
       </c>
       <c r="Q10" s="31"/>
       <c r="R10" s="31"/>
       <c r="S10" s="32"/>
-      <c r="T10" s="69" t="s">
+      <c r="T10" s="82" t="s">
         <v>120</v>
       </c>
-      <c r="U10" s="70"/>
-      <c r="V10" s="70"/>
-      <c r="W10" s="70"/>
-      <c r="X10" s="70"/>
-      <c r="Y10" s="71"/>
+      <c r="U10" s="83"/>
+      <c r="V10" s="83"/>
+      <c r="W10" s="83"/>
+      <c r="X10" s="83"/>
+      <c r="Y10" s="84"/>
       <c r="Z10" s="13"/>
     </row>
     <row r="11" spans="1:26" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3771,70 +3771,70 @@
     </row>
     <row r="12" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
-      <c r="B12" s="72" t="s">
+      <c r="B12" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="73" t="s">
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="73" t="s">
+      <c r="L12" s="45"/>
+      <c r="M12" s="45"/>
+      <c r="N12" s="45"/>
+      <c r="O12" s="45"/>
+      <c r="P12" s="45"/>
+      <c r="Q12" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="R12" s="39"/>
-      <c r="S12" s="39"/>
-      <c r="T12" s="39"/>
-      <c r="U12" s="39"/>
-      <c r="V12" s="39"/>
-      <c r="W12" s="39"/>
-      <c r="X12" s="39"/>
-      <c r="Y12" s="39"/>
+      <c r="R12" s="45"/>
+      <c r="S12" s="45"/>
+      <c r="T12" s="45"/>
+      <c r="U12" s="45"/>
+      <c r="V12" s="45"/>
+      <c r="W12" s="45"/>
+      <c r="X12" s="45"/>
+      <c r="Y12" s="45"/>
       <c r="Z12" s="14"/>
     </row>
     <row r="13" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="81" t="s">
         <v>114</v>
       </c>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="54">
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="81">
         <v>3228485083</v>
       </c>
-      <c r="L13" s="55"/>
-      <c r="M13" s="55"/>
-      <c r="N13" s="55"/>
-      <c r="O13" s="55"/>
-      <c r="P13" s="56"/>
-      <c r="Q13" s="63" t="s">
+      <c r="L13" s="62"/>
+      <c r="M13" s="62"/>
+      <c r="N13" s="62"/>
+      <c r="O13" s="62"/>
+      <c r="P13" s="63"/>
+      <c r="Q13" s="54" t="s">
         <v>115</v>
       </c>
-      <c r="R13" s="55"/>
-      <c r="S13" s="55"/>
-      <c r="T13" s="55"/>
-      <c r="U13" s="55"/>
-      <c r="V13" s="55"/>
-      <c r="W13" s="55"/>
-      <c r="X13" s="55"/>
-      <c r="Y13" s="56"/>
+      <c r="R13" s="62"/>
+      <c r="S13" s="62"/>
+      <c r="T13" s="62"/>
+      <c r="U13" s="62"/>
+      <c r="V13" s="62"/>
+      <c r="W13" s="62"/>
+      <c r="X13" s="62"/>
+      <c r="Y13" s="63"/>
       <c r="Z13" s="13"/>
     </row>
     <row r="14" spans="1:26" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3867,104 +3867,104 @@
     </row>
     <row r="15" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
-      <c r="B15" s="64" t="s">
+      <c r="B15" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="42"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="42"/>
-      <c r="N15" s="42"/>
-      <c r="O15" s="42"/>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="42"/>
-      <c r="S15" s="42"/>
-      <c r="T15" s="42"/>
-      <c r="U15" s="42"/>
-      <c r="V15" s="42"/>
-      <c r="W15" s="42"/>
-      <c r="X15" s="42"/>
-      <c r="Y15" s="42"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="38"/>
+      <c r="R15" s="38"/>
+      <c r="S15" s="38"/>
+      <c r="T15" s="38"/>
+      <c r="U15" s="38"/>
+      <c r="V15" s="38"/>
+      <c r="W15" s="38"/>
+      <c r="X15" s="38"/>
+      <c r="Y15" s="38"/>
       <c r="Z15" s="13"/>
     </row>
     <row r="16" spans="1:26" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="65" t="s">
+      <c r="C16" s="36"/>
+      <c r="D16" s="90" t="s">
         <v>116</v>
       </c>
-      <c r="E16" s="59" t="s">
+      <c r="E16" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="F16" s="37"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="59" t="s">
+      <c r="F16" s="36"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="I16" s="37"/>
-      <c r="J16" s="57"/>
-      <c r="K16" s="59" t="s">
+      <c r="I16" s="36"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="L16" s="36"/>
-      <c r="M16" s="37"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="59" t="s">
+      <c r="L16" s="35"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="50"/>
+      <c r="O16" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="P16" s="36"/>
-      <c r="Q16" s="37"/>
-      <c r="R16" s="57"/>
-      <c r="S16" s="59" t="s">
+      <c r="P16" s="35"/>
+      <c r="Q16" s="36"/>
+      <c r="R16" s="50"/>
+      <c r="S16" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="T16" s="37"/>
-      <c r="U16" s="57"/>
-      <c r="V16" s="59" t="s">
+      <c r="T16" s="36"/>
+      <c r="U16" s="50"/>
+      <c r="V16" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="W16" s="36"/>
-      <c r="X16" s="37"/>
-      <c r="Y16" s="67"/>
+      <c r="W16" s="35"/>
+      <c r="X16" s="36"/>
+      <c r="Y16" s="92"/>
       <c r="Z16" s="13"/>
     </row>
     <row r="17" spans="1:26" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="58"/>
-      <c r="K17" s="41"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="43"/>
-      <c r="N17" s="58"/>
-      <c r="O17" s="41"/>
-      <c r="P17" s="42"/>
-      <c r="Q17" s="43"/>
-      <c r="R17" s="58"/>
-      <c r="S17" s="41"/>
-      <c r="T17" s="43"/>
-      <c r="U17" s="58"/>
-      <c r="V17" s="41"/>
-      <c r="W17" s="42"/>
-      <c r="X17" s="43"/>
-      <c r="Y17" s="58"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="91"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="51"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="39"/>
+      <c r="R17" s="51"/>
+      <c r="S17" s="37"/>
+      <c r="T17" s="39"/>
+      <c r="U17" s="51"/>
+      <c r="V17" s="37"/>
+      <c r="W17" s="38"/>
+      <c r="X17" s="39"/>
+      <c r="Y17" s="51"/>
       <c r="Z17" s="13"/>
     </row>
     <row r="18" spans="1:26" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3997,7 +3997,7 @@
     </row>
     <row r="19" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="53" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="31"/>
@@ -4007,21 +4007,21 @@
       <c r="G19" s="31"/>
       <c r="H19" s="31"/>
       <c r="I19" s="31"/>
-      <c r="J19" s="60" t="s">
+      <c r="J19" s="53" t="s">
         <v>74</v>
       </c>
       <c r="K19" s="31"/>
       <c r="L19" s="31"/>
       <c r="M19" s="31"/>
       <c r="N19" s="32"/>
-      <c r="O19" s="60" t="s">
+      <c r="O19" s="53" t="s">
         <v>22</v>
       </c>
       <c r="P19" s="31"/>
       <c r="Q19" s="31"/>
       <c r="R19" s="31"/>
       <c r="S19" s="32"/>
-      <c r="T19" s="60" t="s">
+      <c r="T19" s="53" t="s">
         <v>33</v>
       </c>
       <c r="U19" s="31"/>
@@ -4033,38 +4033,38 @@
     </row>
     <row r="20" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
-      <c r="B20" s="90" t="s">
+      <c r="B20" s="59" t="s">
         <v>117</v>
       </c>
-      <c r="C20" s="91"/>
-      <c r="D20" s="91"/>
-      <c r="E20" s="91"/>
-      <c r="F20" s="91"/>
-      <c r="G20" s="91"/>
-      <c r="H20" s="91"/>
-      <c r="I20" s="91"/>
-      <c r="J20" s="92">
+      <c r="C20" s="60"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="60"/>
+      <c r="J20" s="61">
         <v>1099737501</v>
       </c>
-      <c r="K20" s="55"/>
-      <c r="L20" s="55"/>
-      <c r="M20" s="55"/>
-      <c r="N20" s="56"/>
-      <c r="O20" s="54">
+      <c r="K20" s="62"/>
+      <c r="L20" s="62"/>
+      <c r="M20" s="62"/>
+      <c r="N20" s="63"/>
+      <c r="O20" s="81">
         <v>3186040819</v>
       </c>
-      <c r="P20" s="61"/>
-      <c r="Q20" s="61"/>
-      <c r="R20" s="61"/>
-      <c r="S20" s="62"/>
-      <c r="T20" s="63" t="s">
+      <c r="P20" s="55"/>
+      <c r="Q20" s="55"/>
+      <c r="R20" s="55"/>
+      <c r="S20" s="56"/>
+      <c r="T20" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="U20" s="61"/>
-      <c r="V20" s="61"/>
-      <c r="W20" s="61"/>
-      <c r="X20" s="61"/>
-      <c r="Y20" s="62"/>
+      <c r="U20" s="55"/>
+      <c r="V20" s="55"/>
+      <c r="W20" s="55"/>
+      <c r="X20" s="55"/>
+      <c r="Y20" s="56"/>
       <c r="Z20" s="13"/>
     </row>
     <row r="21" spans="1:26" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4097,7 +4097,7 @@
     </row>
     <row r="22" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
-      <c r="B22" s="60" t="s">
+      <c r="B22" s="53" t="s">
         <v>36</v>
       </c>
       <c r="C22" s="31"/>
@@ -4108,7 +4108,7 @@
       <c r="H22" s="31"/>
       <c r="I22" s="31"/>
       <c r="J22" s="32"/>
-      <c r="K22" s="68" t="s">
+      <c r="K22" s="57" t="s">
         <v>38</v>
       </c>
       <c r="L22" s="31"/>
@@ -4129,7 +4129,7 @@
     </row>
     <row r="23" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
-      <c r="B23" s="89">
+      <c r="B23" s="58">
         <v>2673126</v>
       </c>
       <c r="C23" s="31"/>
@@ -4140,7 +4140,7 @@
       <c r="H23" s="31"/>
       <c r="I23" s="31"/>
       <c r="J23" s="32"/>
-      <c r="K23" s="89" t="s">
+      <c r="K23" s="58" t="s">
         <v>119</v>
       </c>
       <c r="L23" s="31"/>
@@ -4189,7 +4189,7 @@
     </row>
     <row r="25" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13"/>
-      <c r="B25" s="68" t="s">
+      <c r="B25" s="57" t="s">
         <v>75</v>
       </c>
       <c r="C25" s="31"/>
@@ -4200,15 +4200,15 @@
       <c r="H25" s="31"/>
       <c r="I25" s="31"/>
       <c r="J25" s="32"/>
-      <c r="K25" s="68" t="s">
+      <c r="K25" s="57" t="s">
         <v>76</v>
       </c>
       <c r="L25" s="31"/>
-      <c r="M25" s="68" t="s">
+      <c r="M25" s="57" t="s">
         <v>77</v>
       </c>
       <c r="N25" s="31"/>
-      <c r="O25" s="68" t="s">
+      <c r="O25" s="57" t="s">
         <v>78</v>
       </c>
       <c r="P25" s="31"/>
@@ -4216,7 +4216,7 @@
       <c r="R25" s="31"/>
       <c r="S25" s="31"/>
       <c r="T25" s="32"/>
-      <c r="U25" s="68" t="s">
+      <c r="U25" s="57" t="s">
         <v>79</v>
       </c>
       <c r="V25" s="31"/>
@@ -4227,498 +4227,498 @@
     </row>
     <row r="26" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
-      <c r="B26" s="50" t="s">
+      <c r="B26" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="51">
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="65">
         <v>45566</v>
       </c>
-      <c r="L26" s="36"/>
-      <c r="M26" s="51">
+      <c r="L26" s="35"/>
+      <c r="M26" s="65">
         <v>45569</v>
       </c>
-      <c r="N26" s="36"/>
-      <c r="O26" s="50"/>
-      <c r="P26" s="36"/>
-      <c r="Q26" s="36"/>
-      <c r="R26" s="36"/>
-      <c r="S26" s="36"/>
-      <c r="T26" s="37"/>
-      <c r="U26" s="50"/>
-      <c r="V26" s="36"/>
-      <c r="W26" s="36"/>
-      <c r="X26" s="36"/>
-      <c r="Y26" s="37"/>
+      <c r="N26" s="35"/>
+      <c r="O26" s="64"/>
+      <c r="P26" s="35"/>
+      <c r="Q26" s="35"/>
+      <c r="R26" s="35"/>
+      <c r="S26" s="35"/>
+      <c r="T26" s="36"/>
+      <c r="U26" s="64"/>
+      <c r="V26" s="35"/>
+      <c r="W26" s="35"/>
+      <c r="X26" s="35"/>
+      <c r="Y26" s="36"/>
       <c r="Z26" s="13"/>
     </row>
     <row r="27" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
-      <c r="B27" s="41"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="41"/>
-      <c r="L27" s="42"/>
-      <c r="M27" s="41"/>
-      <c r="N27" s="42"/>
-      <c r="O27" s="41"/>
-      <c r="P27" s="42"/>
-      <c r="Q27" s="42"/>
-      <c r="R27" s="42"/>
-      <c r="S27" s="42"/>
-      <c r="T27" s="43"/>
-      <c r="U27" s="41"/>
-      <c r="V27" s="42"/>
-      <c r="W27" s="42"/>
-      <c r="X27" s="42"/>
-      <c r="Y27" s="43"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="38"/>
+      <c r="M27" s="37"/>
+      <c r="N27" s="38"/>
+      <c r="O27" s="37"/>
+      <c r="P27" s="38"/>
+      <c r="Q27" s="38"/>
+      <c r="R27" s="38"/>
+      <c r="S27" s="38"/>
+      <c r="T27" s="39"/>
+      <c r="U27" s="37"/>
+      <c r="V27" s="38"/>
+      <c r="W27" s="38"/>
+      <c r="X27" s="38"/>
+      <c r="Y27" s="39"/>
       <c r="Z27" s="13"/>
     </row>
     <row r="28" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
-      <c r="B28" s="50" t="s">
+      <c r="B28" s="64" t="s">
         <v>122</v>
       </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="51">
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="65">
         <v>45572</v>
       </c>
-      <c r="L28" s="36"/>
-      <c r="M28" s="51">
+      <c r="L28" s="35"/>
+      <c r="M28" s="65">
         <v>45574</v>
       </c>
-      <c r="N28" s="36"/>
-      <c r="O28" s="50"/>
-      <c r="P28" s="36"/>
-      <c r="Q28" s="36"/>
-      <c r="R28" s="36"/>
-      <c r="S28" s="36"/>
-      <c r="T28" s="37"/>
-      <c r="U28" s="50"/>
-      <c r="V28" s="36"/>
-      <c r="W28" s="36"/>
-      <c r="X28" s="36"/>
-      <c r="Y28" s="37"/>
+      <c r="N28" s="35"/>
+      <c r="O28" s="64"/>
+      <c r="P28" s="35"/>
+      <c r="Q28" s="35"/>
+      <c r="R28" s="35"/>
+      <c r="S28" s="35"/>
+      <c r="T28" s="36"/>
+      <c r="U28" s="64"/>
+      <c r="V28" s="35"/>
+      <c r="W28" s="35"/>
+      <c r="X28" s="35"/>
+      <c r="Y28" s="36"/>
       <c r="Z28" s="13"/>
     </row>
     <row r="29" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
-      <c r="B29" s="41"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="42"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="41"/>
-      <c r="L29" s="42"/>
-      <c r="M29" s="41"/>
-      <c r="N29" s="42"/>
-      <c r="O29" s="41"/>
-      <c r="P29" s="42"/>
-      <c r="Q29" s="42"/>
-      <c r="R29" s="42"/>
-      <c r="S29" s="42"/>
-      <c r="T29" s="43"/>
-      <c r="U29" s="41"/>
-      <c r="V29" s="42"/>
-      <c r="W29" s="42"/>
-      <c r="X29" s="42"/>
-      <c r="Y29" s="43"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="37"/>
+      <c r="L29" s="38"/>
+      <c r="M29" s="37"/>
+      <c r="N29" s="38"/>
+      <c r="O29" s="37"/>
+      <c r="P29" s="38"/>
+      <c r="Q29" s="38"/>
+      <c r="R29" s="38"/>
+      <c r="S29" s="38"/>
+      <c r="T29" s="39"/>
+      <c r="U29" s="37"/>
+      <c r="V29" s="38"/>
+      <c r="W29" s="38"/>
+      <c r="X29" s="38"/>
+      <c r="Y29" s="39"/>
       <c r="Z29" s="13"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
-      <c r="B30" s="50" t="s">
+      <c r="B30" s="64" t="s">
         <v>123</v>
       </c>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="51">
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="65">
         <v>45575</v>
       </c>
-      <c r="L30" s="36"/>
-      <c r="M30" s="51">
+      <c r="L30" s="35"/>
+      <c r="M30" s="65">
         <v>45580</v>
       </c>
-      <c r="N30" s="36"/>
-      <c r="O30" s="50"/>
-      <c r="P30" s="36"/>
-      <c r="Q30" s="36"/>
-      <c r="R30" s="36"/>
-      <c r="S30" s="36"/>
-      <c r="T30" s="37"/>
-      <c r="U30" s="50"/>
-      <c r="V30" s="36"/>
-      <c r="W30" s="36"/>
-      <c r="X30" s="36"/>
-      <c r="Y30" s="37"/>
+      <c r="N30" s="35"/>
+      <c r="O30" s="64"/>
+      <c r="P30" s="35"/>
+      <c r="Q30" s="35"/>
+      <c r="R30" s="35"/>
+      <c r="S30" s="35"/>
+      <c r="T30" s="36"/>
+      <c r="U30" s="64"/>
+      <c r="V30" s="35"/>
+      <c r="W30" s="35"/>
+      <c r="X30" s="35"/>
+      <c r="Y30" s="36"/>
       <c r="Z30" s="13"/>
     </row>
     <row r="31" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
-      <c r="B31" s="41"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="41"/>
-      <c r="L31" s="42"/>
-      <c r="M31" s="41"/>
-      <c r="N31" s="42"/>
-      <c r="O31" s="41"/>
-      <c r="P31" s="42"/>
-      <c r="Q31" s="42"/>
-      <c r="R31" s="42"/>
-      <c r="S31" s="42"/>
-      <c r="T31" s="43"/>
-      <c r="U31" s="41"/>
-      <c r="V31" s="42"/>
-      <c r="W31" s="42"/>
-      <c r="X31" s="42"/>
-      <c r="Y31" s="43"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="37"/>
+      <c r="L31" s="38"/>
+      <c r="M31" s="37"/>
+      <c r="N31" s="38"/>
+      <c r="O31" s="37"/>
+      <c r="P31" s="38"/>
+      <c r="Q31" s="38"/>
+      <c r="R31" s="38"/>
+      <c r="S31" s="38"/>
+      <c r="T31" s="39"/>
+      <c r="U31" s="37"/>
+      <c r="V31" s="38"/>
+      <c r="W31" s="38"/>
+      <c r="X31" s="38"/>
+      <c r="Y31" s="39"/>
       <c r="Z31" s="13"/>
     </row>
     <row r="32" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
-      <c r="B32" s="50"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="51"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="51"/>
-      <c r="N32" s="36"/>
-      <c r="O32" s="50"/>
-      <c r="P32" s="36"/>
-      <c r="Q32" s="36"/>
-      <c r="R32" s="36"/>
-      <c r="S32" s="36"/>
-      <c r="T32" s="37"/>
-      <c r="U32" s="50"/>
-      <c r="V32" s="36"/>
-      <c r="W32" s="36"/>
-      <c r="X32" s="36"/>
-      <c r="Y32" s="37"/>
+      <c r="B32" s="64"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="36"/>
+      <c r="K32" s="65"/>
+      <c r="L32" s="35"/>
+      <c r="M32" s="65"/>
+      <c r="N32" s="35"/>
+      <c r="O32" s="64"/>
+      <c r="P32" s="35"/>
+      <c r="Q32" s="35"/>
+      <c r="R32" s="35"/>
+      <c r="S32" s="35"/>
+      <c r="T32" s="36"/>
+      <c r="U32" s="64"/>
+      <c r="V32" s="35"/>
+      <c r="W32" s="35"/>
+      <c r="X32" s="35"/>
+      <c r="Y32" s="36"/>
       <c r="Z32" s="13"/>
     </row>
     <row r="33" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="42"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="42"/>
-      <c r="I33" s="42"/>
-      <c r="J33" s="43"/>
-      <c r="K33" s="41"/>
-      <c r="L33" s="42"/>
-      <c r="M33" s="41"/>
-      <c r="N33" s="42"/>
-      <c r="O33" s="41"/>
-      <c r="P33" s="42"/>
-      <c r="Q33" s="42"/>
-      <c r="R33" s="42"/>
-      <c r="S33" s="42"/>
-      <c r="T33" s="43"/>
-      <c r="U33" s="41"/>
-      <c r="V33" s="42"/>
-      <c r="W33" s="42"/>
-      <c r="X33" s="42"/>
-      <c r="Y33" s="43"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="37"/>
+      <c r="L33" s="38"/>
+      <c r="M33" s="37"/>
+      <c r="N33" s="38"/>
+      <c r="O33" s="37"/>
+      <c r="P33" s="38"/>
+      <c r="Q33" s="38"/>
+      <c r="R33" s="38"/>
+      <c r="S33" s="38"/>
+      <c r="T33" s="39"/>
+      <c r="U33" s="37"/>
+      <c r="V33" s="38"/>
+      <c r="W33" s="38"/>
+      <c r="X33" s="38"/>
+      <c r="Y33" s="39"/>
       <c r="Z33" s="13"/>
     </row>
     <row r="34" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
-      <c r="B34" s="50"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="37"/>
-      <c r="K34" s="51"/>
-      <c r="L34" s="36"/>
-      <c r="M34" s="51"/>
-      <c r="N34" s="36"/>
-      <c r="O34" s="50"/>
-      <c r="P34" s="36"/>
-      <c r="Q34" s="36"/>
-      <c r="R34" s="36"/>
-      <c r="S34" s="36"/>
-      <c r="T34" s="37"/>
-      <c r="U34" s="50"/>
-      <c r="V34" s="36"/>
-      <c r="W34" s="36"/>
-      <c r="X34" s="36"/>
-      <c r="Y34" s="37"/>
+      <c r="B34" s="64"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="36"/>
+      <c r="K34" s="65"/>
+      <c r="L34" s="35"/>
+      <c r="M34" s="65"/>
+      <c r="N34" s="35"/>
+      <c r="O34" s="64"/>
+      <c r="P34" s="35"/>
+      <c r="Q34" s="35"/>
+      <c r="R34" s="35"/>
+      <c r="S34" s="35"/>
+      <c r="T34" s="36"/>
+      <c r="U34" s="64"/>
+      <c r="V34" s="35"/>
+      <c r="W34" s="35"/>
+      <c r="X34" s="35"/>
+      <c r="Y34" s="36"/>
       <c r="Z34" s="13"/>
     </row>
     <row r="35" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
-      <c r="B35" s="41"/>
-      <c r="C35" s="42"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="42"/>
-      <c r="H35" s="42"/>
-      <c r="I35" s="42"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="41"/>
-      <c r="L35" s="42"/>
-      <c r="M35" s="41"/>
-      <c r="N35" s="42"/>
-      <c r="O35" s="41"/>
-      <c r="P35" s="42"/>
-      <c r="Q35" s="42"/>
-      <c r="R35" s="42"/>
-      <c r="S35" s="42"/>
-      <c r="T35" s="43"/>
-      <c r="U35" s="41"/>
-      <c r="V35" s="42"/>
-      <c r="W35" s="42"/>
-      <c r="X35" s="42"/>
-      <c r="Y35" s="43"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="38"/>
+      <c r="M35" s="37"/>
+      <c r="N35" s="38"/>
+      <c r="O35" s="37"/>
+      <c r="P35" s="38"/>
+      <c r="Q35" s="38"/>
+      <c r="R35" s="38"/>
+      <c r="S35" s="38"/>
+      <c r="T35" s="39"/>
+      <c r="U35" s="37"/>
+      <c r="V35" s="38"/>
+      <c r="W35" s="38"/>
+      <c r="X35" s="38"/>
+      <c r="Y35" s="39"/>
       <c r="Z35" s="13"/>
     </row>
     <row r="36" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
-      <c r="B36" s="50"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="37"/>
-      <c r="K36" s="51"/>
-      <c r="L36" s="36"/>
-      <c r="M36" s="51"/>
-      <c r="N36" s="36"/>
-      <c r="O36" s="50"/>
-      <c r="P36" s="36"/>
-      <c r="Q36" s="36"/>
-      <c r="R36" s="36"/>
-      <c r="S36" s="36"/>
-      <c r="T36" s="37"/>
-      <c r="U36" s="50"/>
-      <c r="V36" s="36"/>
-      <c r="W36" s="36"/>
-      <c r="X36" s="36"/>
-      <c r="Y36" s="37"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="65"/>
+      <c r="L36" s="35"/>
+      <c r="M36" s="65"/>
+      <c r="N36" s="35"/>
+      <c r="O36" s="64"/>
+      <c r="P36" s="35"/>
+      <c r="Q36" s="35"/>
+      <c r="R36" s="35"/>
+      <c r="S36" s="35"/>
+      <c r="T36" s="36"/>
+      <c r="U36" s="64"/>
+      <c r="V36" s="35"/>
+      <c r="W36" s="35"/>
+      <c r="X36" s="35"/>
+      <c r="Y36" s="36"/>
       <c r="Z36" s="13"/>
     </row>
     <row r="37" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
-      <c r="B37" s="41"/>
-      <c r="C37" s="42"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="42"/>
-      <c r="G37" s="42"/>
-      <c r="H37" s="42"/>
-      <c r="I37" s="42"/>
-      <c r="J37" s="43"/>
-      <c r="K37" s="41"/>
-      <c r="L37" s="42"/>
-      <c r="M37" s="41"/>
-      <c r="N37" s="42"/>
-      <c r="O37" s="41"/>
-      <c r="P37" s="42"/>
-      <c r="Q37" s="42"/>
-      <c r="R37" s="42"/>
-      <c r="S37" s="42"/>
-      <c r="T37" s="43"/>
-      <c r="U37" s="41"/>
-      <c r="V37" s="42"/>
-      <c r="W37" s="42"/>
-      <c r="X37" s="42"/>
-      <c r="Y37" s="43"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="38"/>
+      <c r="M37" s="37"/>
+      <c r="N37" s="38"/>
+      <c r="O37" s="37"/>
+      <c r="P37" s="38"/>
+      <c r="Q37" s="38"/>
+      <c r="R37" s="38"/>
+      <c r="S37" s="38"/>
+      <c r="T37" s="39"/>
+      <c r="U37" s="37"/>
+      <c r="V37" s="38"/>
+      <c r="W37" s="38"/>
+      <c r="X37" s="38"/>
+      <c r="Y37" s="39"/>
       <c r="Z37" s="13"/>
     </row>
     <row r="38" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
-      <c r="B38" s="50"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="37"/>
-      <c r="K38" s="51"/>
-      <c r="L38" s="36"/>
-      <c r="M38" s="51"/>
-      <c r="N38" s="36"/>
-      <c r="O38" s="50"/>
-      <c r="P38" s="36"/>
-      <c r="Q38" s="36"/>
-      <c r="R38" s="36"/>
-      <c r="S38" s="36"/>
-      <c r="T38" s="37"/>
-      <c r="U38" s="50"/>
-      <c r="V38" s="36"/>
-      <c r="W38" s="36"/>
-      <c r="X38" s="36"/>
-      <c r="Y38" s="37"/>
+      <c r="B38" s="64"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="36"/>
+      <c r="K38" s="65"/>
+      <c r="L38" s="35"/>
+      <c r="M38" s="65"/>
+      <c r="N38" s="35"/>
+      <c r="O38" s="64"/>
+      <c r="P38" s="35"/>
+      <c r="Q38" s="35"/>
+      <c r="R38" s="35"/>
+      <c r="S38" s="35"/>
+      <c r="T38" s="36"/>
+      <c r="U38" s="64"/>
+      <c r="V38" s="35"/>
+      <c r="W38" s="35"/>
+      <c r="X38" s="35"/>
+      <c r="Y38" s="36"/>
       <c r="Z38" s="13"/>
     </row>
     <row r="39" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
-      <c r="B39" s="41"/>
-      <c r="C39" s="42"/>
-      <c r="D39" s="42"/>
-      <c r="E39" s="42"/>
-      <c r="F39" s="42"/>
-      <c r="G39" s="42"/>
-      <c r="H39" s="42"/>
-      <c r="I39" s="42"/>
-      <c r="J39" s="43"/>
-      <c r="K39" s="41"/>
-      <c r="L39" s="42"/>
-      <c r="M39" s="41"/>
-      <c r="N39" s="42"/>
-      <c r="O39" s="41"/>
-      <c r="P39" s="42"/>
-      <c r="Q39" s="42"/>
-      <c r="R39" s="42"/>
-      <c r="S39" s="42"/>
-      <c r="T39" s="43"/>
-      <c r="U39" s="41"/>
-      <c r="V39" s="42"/>
-      <c r="W39" s="42"/>
-      <c r="X39" s="42"/>
-      <c r="Y39" s="43"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="37"/>
+      <c r="L39" s="38"/>
+      <c r="M39" s="37"/>
+      <c r="N39" s="38"/>
+      <c r="O39" s="37"/>
+      <c r="P39" s="38"/>
+      <c r="Q39" s="38"/>
+      <c r="R39" s="38"/>
+      <c r="S39" s="38"/>
+      <c r="T39" s="39"/>
+      <c r="U39" s="37"/>
+      <c r="V39" s="38"/>
+      <c r="W39" s="38"/>
+      <c r="X39" s="38"/>
+      <c r="Y39" s="39"/>
       <c r="Z39" s="13"/>
     </row>
     <row r="40" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
-      <c r="B40" s="50"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="37"/>
-      <c r="K40" s="51"/>
-      <c r="L40" s="36"/>
-      <c r="M40" s="51"/>
-      <c r="N40" s="36"/>
-      <c r="O40" s="50"/>
-      <c r="P40" s="36"/>
-      <c r="Q40" s="36"/>
-      <c r="R40" s="36"/>
-      <c r="S40" s="36"/>
-      <c r="T40" s="37"/>
-      <c r="U40" s="50"/>
-      <c r="V40" s="36"/>
-      <c r="W40" s="36"/>
-      <c r="X40" s="36"/>
-      <c r="Y40" s="37"/>
+      <c r="B40" s="64"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="35"/>
+      <c r="J40" s="36"/>
+      <c r="K40" s="65"/>
+      <c r="L40" s="35"/>
+      <c r="M40" s="65"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="64"/>
+      <c r="P40" s="35"/>
+      <c r="Q40" s="35"/>
+      <c r="R40" s="35"/>
+      <c r="S40" s="35"/>
+      <c r="T40" s="36"/>
+      <c r="U40" s="64"/>
+      <c r="V40" s="35"/>
+      <c r="W40" s="35"/>
+      <c r="X40" s="35"/>
+      <c r="Y40" s="36"/>
       <c r="Z40" s="13"/>
     </row>
     <row r="41" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
-      <c r="B41" s="41"/>
-      <c r="C41" s="42"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="42"/>
-      <c r="J41" s="43"/>
-      <c r="K41" s="41"/>
-      <c r="L41" s="42"/>
-      <c r="M41" s="41"/>
-      <c r="N41" s="42"/>
-      <c r="O41" s="41"/>
-      <c r="P41" s="42"/>
-      <c r="Q41" s="42"/>
-      <c r="R41" s="42"/>
-      <c r="S41" s="42"/>
-      <c r="T41" s="43"/>
-      <c r="U41" s="41"/>
-      <c r="V41" s="42"/>
-      <c r="W41" s="42"/>
-      <c r="X41" s="42"/>
-      <c r="Y41" s="43"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="37"/>
+      <c r="L41" s="38"/>
+      <c r="M41" s="37"/>
+      <c r="N41" s="38"/>
+      <c r="O41" s="37"/>
+      <c r="P41" s="38"/>
+      <c r="Q41" s="38"/>
+      <c r="R41" s="38"/>
+      <c r="S41" s="38"/>
+      <c r="T41" s="39"/>
+      <c r="U41" s="37"/>
+      <c r="V41" s="38"/>
+      <c r="W41" s="38"/>
+      <c r="X41" s="38"/>
+      <c r="Y41" s="39"/>
       <c r="Z41" s="13"/>
     </row>
     <row r="42" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
-      <c r="B42" s="87" t="s">
+      <c r="B42" s="70" t="s">
         <v>80</v>
       </c>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="36"/>
-      <c r="K42" s="36"/>
-      <c r="L42" s="36"/>
-      <c r="M42" s="36"/>
-      <c r="N42" s="36"/>
-      <c r="O42" s="36"/>
-      <c r="P42" s="36"/>
-      <c r="Q42" s="36"/>
-      <c r="R42" s="36"/>
-      <c r="S42" s="36"/>
-      <c r="T42" s="36"/>
-      <c r="U42" s="36"/>
-      <c r="V42" s="36"/>
-      <c r="W42" s="36"/>
-      <c r="X42" s="36"/>
-      <c r="Y42" s="36"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="35"/>
+      <c r="G42" s="35"/>
+      <c r="H42" s="35"/>
+      <c r="I42" s="35"/>
+      <c r="J42" s="35"/>
+      <c r="K42" s="35"/>
+      <c r="L42" s="35"/>
+      <c r="M42" s="35"/>
+      <c r="N42" s="35"/>
+      <c r="O42" s="35"/>
+      <c r="P42" s="35"/>
+      <c r="Q42" s="35"/>
+      <c r="R42" s="35"/>
+      <c r="S42" s="35"/>
+      <c r="T42" s="35"/>
+      <c r="U42" s="35"/>
+      <c r="V42" s="35"/>
+      <c r="W42" s="35"/>
+      <c r="X42" s="35"/>
+      <c r="Y42" s="35"/>
       <c r="Z42" s="13"/>
     </row>
     <row r="43" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4780,14 +4780,14 @@
     <row r="45" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
       <c r="B45" s="20"/>
-      <c r="C45" s="52" t="s">
+      <c r="C45" s="87" t="s">
         <v>117</v>
       </c>
-      <c r="D45" s="52"/>
-      <c r="E45" s="52"/>
-      <c r="F45" s="52"/>
-      <c r="G45" s="52"/>
-      <c r="H45" s="52"/>
+      <c r="D45" s="87"/>
+      <c r="E45" s="87"/>
+      <c r="F45" s="87"/>
+      <c r="G45" s="87"/>
+      <c r="H45" s="87"/>
       <c r="I45" s="20"/>
       <c r="J45" s="21"/>
       <c r="K45" s="21"/>
@@ -4800,46 +4800,46 @@
       <c r="R45" s="21"/>
       <c r="S45" s="16"/>
       <c r="T45" s="22"/>
-      <c r="U45" s="53">
-        <v>45580</v>
+      <c r="U45" s="88">
+        <v>45581</v>
       </c>
-      <c r="V45" s="53"/>
-      <c r="W45" s="53"/>
+      <c r="V45" s="88"/>
+      <c r="W45" s="88"/>
       <c r="X45" s="22"/>
       <c r="Y45" s="16"/>
       <c r="Z45" s="13"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
-      <c r="B46" s="88" t="s">
+      <c r="B46" s="71" t="s">
         <v>81</v>
       </c>
-      <c r="C46" s="39"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="39"/>
-      <c r="G46" s="39"/>
-      <c r="H46" s="39"/>
-      <c r="I46" s="39"/>
+      <c r="C46" s="45"/>
+      <c r="D46" s="45"/>
+      <c r="E46" s="45"/>
+      <c r="F46" s="45"/>
+      <c r="G46" s="45"/>
+      <c r="H46" s="45"/>
+      <c r="I46" s="45"/>
       <c r="J46" s="21"/>
-      <c r="K46" s="83" t="s">
+      <c r="K46" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="L46" s="36"/>
-      <c r="M46" s="36"/>
-      <c r="N46" s="36"/>
-      <c r="O46" s="36"/>
-      <c r="P46" s="36"/>
-      <c r="Q46" s="36"/>
+      <c r="L46" s="35"/>
+      <c r="M46" s="35"/>
+      <c r="N46" s="35"/>
+      <c r="O46" s="35"/>
+      <c r="P46" s="35"/>
+      <c r="Q46" s="35"/>
       <c r="R46" s="24"/>
       <c r="S46" s="21"/>
-      <c r="T46" s="88" t="s">
+      <c r="T46" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="U46" s="39"/>
-      <c r="V46" s="39"/>
-      <c r="W46" s="39"/>
-      <c r="X46" s="39"/>
+      <c r="U46" s="45"/>
+      <c r="V46" s="45"/>
+      <c r="W46" s="45"/>
+      <c r="X46" s="45"/>
       <c r="Y46" s="21"/>
       <c r="Z46" s="13"/>
     </row>
@@ -4873,14 +4873,14 @@
     </row>
     <row r="48" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
-      <c r="B48" s="88"/>
-      <c r="C48" s="39"/>
-      <c r="D48" s="39"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="39"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="39"/>
-      <c r="I48" s="39"/>
+      <c r="B48" s="71"/>
+      <c r="C48" s="45"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="45"/>
+      <c r="G48" s="45"/>
+      <c r="H48" s="45"/>
+      <c r="I48" s="45"/>
       <c r="J48" s="13"/>
       <c r="K48" s="13"/>
       <c r="L48" s="13"/>
@@ -4931,36 +4931,36 @@
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="13"/>
-      <c r="B50" s="88" t="s">
+      <c r="B50" s="71" t="s">
         <v>83</v>
       </c>
-      <c r="C50" s="39"/>
-      <c r="D50" s="39"/>
-      <c r="E50" s="39"/>
-      <c r="F50" s="39"/>
-      <c r="G50" s="39"/>
-      <c r="H50" s="39"/>
-      <c r="I50" s="39"/>
+      <c r="C50" s="45"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="45"/>
+      <c r="G50" s="45"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="45"/>
       <c r="J50" s="21"/>
-      <c r="K50" s="83" t="s">
+      <c r="K50" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="L50" s="36"/>
-      <c r="M50" s="36"/>
-      <c r="N50" s="36"/>
-      <c r="O50" s="36"/>
-      <c r="P50" s="36"/>
-      <c r="Q50" s="36"/>
+      <c r="L50" s="35"/>
+      <c r="M50" s="35"/>
+      <c r="N50" s="35"/>
+      <c r="O50" s="35"/>
+      <c r="P50" s="35"/>
+      <c r="Q50" s="35"/>
       <c r="R50" s="24"/>
-      <c r="S50" s="84" t="s">
+      <c r="S50" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="T50" s="39"/>
-      <c r="U50" s="39"/>
-      <c r="V50" s="39"/>
-      <c r="W50" s="39"/>
-      <c r="X50" s="39"/>
-      <c r="Y50" s="39"/>
+      <c r="T50" s="45"/>
+      <c r="U50" s="45"/>
+      <c r="V50" s="45"/>
+      <c r="W50" s="45"/>
+      <c r="X50" s="45"/>
+      <c r="Y50" s="45"/>
       <c r="Z50" s="13"/>
     </row>
     <row r="51" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4980,11 +4980,11 @@
       <c r="N51" s="13"/>
       <c r="O51" s="13"/>
       <c r="P51" s="13"/>
-      <c r="Q51" s="85"/>
-      <c r="R51" s="39"/>
-      <c r="S51" s="39"/>
-      <c r="T51" s="39"/>
-      <c r="U51" s="39"/>
+      <c r="Q51" s="68"/>
+      <c r="R51" s="45"/>
+      <c r="S51" s="45"/>
+      <c r="T51" s="45"/>
+      <c r="U51" s="45"/>
       <c r="V51" s="13"/>
       <c r="W51" s="13"/>
       <c r="X51" s="13"/>
@@ -4993,60 +4993,60 @@
     </row>
     <row r="52" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="13"/>
-      <c r="B52" s="86" t="s">
+      <c r="B52" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="C52" s="39"/>
-      <c r="D52" s="39"/>
-      <c r="E52" s="39"/>
-      <c r="F52" s="39"/>
-      <c r="G52" s="39"/>
-      <c r="H52" s="39"/>
-      <c r="I52" s="39"/>
-      <c r="J52" s="39"/>
-      <c r="K52" s="39"/>
-      <c r="L52" s="39"/>
-      <c r="M52" s="39"/>
-      <c r="N52" s="39"/>
-      <c r="O52" s="39"/>
-      <c r="P52" s="39"/>
-      <c r="Q52" s="39"/>
-      <c r="R52" s="39"/>
-      <c r="S52" s="39"/>
-      <c r="T52" s="39"/>
-      <c r="U52" s="39"/>
-      <c r="V52" s="39"/>
-      <c r="W52" s="39"/>
-      <c r="X52" s="39"/>
-      <c r="Y52" s="39"/>
+      <c r="C52" s="45"/>
+      <c r="D52" s="45"/>
+      <c r="E52" s="45"/>
+      <c r="F52" s="45"/>
+      <c r="G52" s="45"/>
+      <c r="H52" s="45"/>
+      <c r="I52" s="45"/>
+      <c r="J52" s="45"/>
+      <c r="K52" s="45"/>
+      <c r="L52" s="45"/>
+      <c r="M52" s="45"/>
+      <c r="N52" s="45"/>
+      <c r="O52" s="45"/>
+      <c r="P52" s="45"/>
+      <c r="Q52" s="45"/>
+      <c r="R52" s="45"/>
+      <c r="S52" s="45"/>
+      <c r="T52" s="45"/>
+      <c r="U52" s="45"/>
+      <c r="V52" s="45"/>
+      <c r="W52" s="45"/>
+      <c r="X52" s="45"/>
+      <c r="Y52" s="45"/>
       <c r="Z52" s="13"/>
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="13"/>
-      <c r="B53" s="39"/>
-      <c r="C53" s="39"/>
-      <c r="D53" s="39"/>
-      <c r="E53" s="39"/>
-      <c r="F53" s="39"/>
-      <c r="G53" s="39"/>
-      <c r="H53" s="39"/>
-      <c r="I53" s="39"/>
-      <c r="J53" s="39"/>
-      <c r="K53" s="39"/>
-      <c r="L53" s="39"/>
-      <c r="M53" s="39"/>
-      <c r="N53" s="39"/>
-      <c r="O53" s="39"/>
-      <c r="P53" s="39"/>
-      <c r="Q53" s="39"/>
-      <c r="R53" s="39"/>
-      <c r="S53" s="39"/>
-      <c r="T53" s="39"/>
-      <c r="U53" s="39"/>
-      <c r="V53" s="39"/>
-      <c r="W53" s="39"/>
-      <c r="X53" s="39"/>
-      <c r="Y53" s="39"/>
+      <c r="B53" s="45"/>
+      <c r="C53" s="45"/>
+      <c r="D53" s="45"/>
+      <c r="E53" s="45"/>
+      <c r="F53" s="45"/>
+      <c r="G53" s="45"/>
+      <c r="H53" s="45"/>
+      <c r="I53" s="45"/>
+      <c r="J53" s="45"/>
+      <c r="K53" s="45"/>
+      <c r="L53" s="45"/>
+      <c r="M53" s="45"/>
+      <c r="N53" s="45"/>
+      <c r="O53" s="45"/>
+      <c r="P53" s="45"/>
+      <c r="Q53" s="45"/>
+      <c r="R53" s="45"/>
+      <c r="S53" s="45"/>
+      <c r="T53" s="45"/>
+      <c r="U53" s="45"/>
+      <c r="V53" s="45"/>
+      <c r="W53" s="45"/>
+      <c r="X53" s="45"/>
+      <c r="Y53" s="45"/>
       <c r="Z53" s="13"/>
     </row>
     <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -31567,19 +31567,76 @@
     </row>
   </sheetData>
   <mergeCells count="107">
-    <mergeCell ref="U16:U17"/>
-    <mergeCell ref="V16:X17"/>
-    <mergeCell ref="T19:Y19"/>
-    <mergeCell ref="T20:Y20"/>
-    <mergeCell ref="K22:Y22"/>
-    <mergeCell ref="K23:Y23"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="K16:M17"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="J19:N19"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="J20:N20"/>
-    <mergeCell ref="B22:J22"/>
+    <mergeCell ref="B28:J29"/>
+    <mergeCell ref="K28:L29"/>
+    <mergeCell ref="M28:N29"/>
+    <mergeCell ref="O28:T29"/>
+    <mergeCell ref="U28:Y29"/>
+    <mergeCell ref="C45:H45"/>
+    <mergeCell ref="U45:W45"/>
+    <mergeCell ref="B13:J13"/>
+    <mergeCell ref="K13:P13"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="O16:Q17"/>
+    <mergeCell ref="O19:S19"/>
+    <mergeCell ref="O20:S20"/>
+    <mergeCell ref="R16:R17"/>
+    <mergeCell ref="S16:T17"/>
+    <mergeCell ref="Q13:Y13"/>
+    <mergeCell ref="B15:Y15"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:I17"/>
+    <mergeCell ref="Y16:Y17"/>
+    <mergeCell ref="B38:J39"/>
+    <mergeCell ref="B9:L9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="P9:S9"/>
+    <mergeCell ref="T9:Y9"/>
+    <mergeCell ref="B10:L10"/>
+    <mergeCell ref="T10:Y10"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="P10:S10"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="K12:P12"/>
+    <mergeCell ref="Q12:Y12"/>
+    <mergeCell ref="B1:V2"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="B3:Y3"/>
+    <mergeCell ref="B4:Y4"/>
+    <mergeCell ref="B5:Y5"/>
+    <mergeCell ref="B6:Y6"/>
+    <mergeCell ref="B7:Y7"/>
+    <mergeCell ref="B8:Y8"/>
+    <mergeCell ref="K50:Q50"/>
+    <mergeCell ref="S50:Y50"/>
+    <mergeCell ref="Q51:U51"/>
+    <mergeCell ref="B52:Y53"/>
+    <mergeCell ref="B40:J41"/>
+    <mergeCell ref="B42:Y42"/>
+    <mergeCell ref="B46:I46"/>
+    <mergeCell ref="K46:Q46"/>
+    <mergeCell ref="T46:X46"/>
+    <mergeCell ref="B48:I48"/>
+    <mergeCell ref="B50:I50"/>
+    <mergeCell ref="M40:N41"/>
+    <mergeCell ref="O40:T41"/>
+    <mergeCell ref="M34:N35"/>
+    <mergeCell ref="K38:L39"/>
+    <mergeCell ref="M38:N39"/>
+    <mergeCell ref="O38:T39"/>
+    <mergeCell ref="U38:Y39"/>
+    <mergeCell ref="K40:L41"/>
+    <mergeCell ref="U40:Y41"/>
+    <mergeCell ref="M32:N33"/>
+    <mergeCell ref="O32:T33"/>
+    <mergeCell ref="O34:T35"/>
+    <mergeCell ref="U34:Y35"/>
+    <mergeCell ref="O36:T37"/>
+    <mergeCell ref="U36:Y37"/>
     <mergeCell ref="B36:J37"/>
     <mergeCell ref="K36:L37"/>
     <mergeCell ref="M36:N37"/>
@@ -31604,76 +31661,19 @@
     <mergeCell ref="B32:J33"/>
     <mergeCell ref="B34:J35"/>
     <mergeCell ref="K34:L35"/>
-    <mergeCell ref="M34:N35"/>
-    <mergeCell ref="K38:L39"/>
-    <mergeCell ref="M38:N39"/>
-    <mergeCell ref="O38:T39"/>
-    <mergeCell ref="U38:Y39"/>
-    <mergeCell ref="K40:L41"/>
-    <mergeCell ref="U40:Y41"/>
-    <mergeCell ref="M32:N33"/>
-    <mergeCell ref="O32:T33"/>
-    <mergeCell ref="O34:T35"/>
-    <mergeCell ref="U34:Y35"/>
-    <mergeCell ref="O36:T37"/>
-    <mergeCell ref="U36:Y37"/>
-    <mergeCell ref="K50:Q50"/>
-    <mergeCell ref="S50:Y50"/>
-    <mergeCell ref="Q51:U51"/>
-    <mergeCell ref="B52:Y53"/>
-    <mergeCell ref="B40:J41"/>
-    <mergeCell ref="B42:Y42"/>
-    <mergeCell ref="B46:I46"/>
-    <mergeCell ref="K46:Q46"/>
-    <mergeCell ref="T46:X46"/>
-    <mergeCell ref="B48:I48"/>
-    <mergeCell ref="B50:I50"/>
-    <mergeCell ref="M40:N41"/>
-    <mergeCell ref="O40:T41"/>
-    <mergeCell ref="B1:V2"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="B3:Y3"/>
-    <mergeCell ref="B4:Y4"/>
-    <mergeCell ref="B5:Y5"/>
-    <mergeCell ref="B6:Y6"/>
-    <mergeCell ref="B7:Y7"/>
-    <mergeCell ref="B8:Y8"/>
-    <mergeCell ref="B9:L9"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="P9:S9"/>
-    <mergeCell ref="T9:Y9"/>
-    <mergeCell ref="B10:L10"/>
-    <mergeCell ref="T10:Y10"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="P10:S10"/>
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="K12:P12"/>
-    <mergeCell ref="Q12:Y12"/>
-    <mergeCell ref="B28:J29"/>
-    <mergeCell ref="K28:L29"/>
-    <mergeCell ref="M28:N29"/>
-    <mergeCell ref="O28:T29"/>
-    <mergeCell ref="U28:Y29"/>
-    <mergeCell ref="C45:H45"/>
-    <mergeCell ref="U45:W45"/>
-    <mergeCell ref="B13:J13"/>
-    <mergeCell ref="K13:P13"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="O16:Q17"/>
-    <mergeCell ref="O19:S19"/>
-    <mergeCell ref="O20:S20"/>
-    <mergeCell ref="R16:R17"/>
-    <mergeCell ref="S16:T17"/>
-    <mergeCell ref="Q13:Y13"/>
-    <mergeCell ref="B15:Y15"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:I17"/>
-    <mergeCell ref="Y16:Y17"/>
-    <mergeCell ref="B38:J39"/>
+    <mergeCell ref="U16:U17"/>
+    <mergeCell ref="V16:X17"/>
+    <mergeCell ref="T19:Y19"/>
+    <mergeCell ref="T20:Y20"/>
+    <mergeCell ref="K22:Y22"/>
+    <mergeCell ref="K23:Y23"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K16:M17"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="J19:N19"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="J20:N20"/>
+    <mergeCell ref="B22:J22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q13" r:id="rId1" xr:uid="{72239C27-A50D-42EF-AE41-9F139FB962F5}"/>
@@ -31699,64 +31699,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="93" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="106" t="s">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="93" t="s">
         <v>87</v>
       </c>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
-      <c r="X1" s="39"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
       <c r="Y1" s="26"/>
       <c r="Z1" s="26"/>
     </row>
     <row r="2" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="106"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="107" t="s">
+      <c r="A2" s="93"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="45"/>
+      <c r="S2" s="45"/>
+      <c r="T2" s="45"/>
+      <c r="U2" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="V2" s="36"/>
-      <c r="W2" s="36"/>
-      <c r="X2" s="36"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
       <c r="Y2" s="26"/>
       <c r="Z2" s="26"/>
     </row>
@@ -31781,70 +31781,70 @@
       <c r="R3" s="26"/>
       <c r="S3" s="26"/>
       <c r="T3" s="26"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="39"/>
-      <c r="W3" s="39"/>
-      <c r="X3" s="39"/>
+      <c r="U3" s="45"/>
+      <c r="V3" s="45"/>
+      <c r="W3" s="45"/>
+      <c r="X3" s="45"/>
       <c r="Y3" s="26"/>
       <c r="Z3" s="26"/>
     </row>
     <row r="4" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="108" t="s">
+      <c r="A4" s="95" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="104"/>
-      <c r="C4" s="104"/>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104"/>
-      <c r="F4" s="104"/>
-      <c r="G4" s="104"/>
-      <c r="H4" s="104"/>
-      <c r="I4" s="104"/>
-      <c r="J4" s="104"/>
-      <c r="K4" s="104"/>
-      <c r="L4" s="104"/>
-      <c r="M4" s="105"/>
-      <c r="N4" s="108" t="s">
+      <c r="B4" s="96"/>
+      <c r="C4" s="96"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="96"/>
+      <c r="F4" s="96"/>
+      <c r="G4" s="96"/>
+      <c r="H4" s="96"/>
+      <c r="I4" s="96"/>
+      <c r="J4" s="96"/>
+      <c r="K4" s="96"/>
+      <c r="L4" s="96"/>
+      <c r="M4" s="97"/>
+      <c r="N4" s="95" t="s">
         <v>90</v>
       </c>
-      <c r="O4" s="104"/>
-      <c r="P4" s="104"/>
-      <c r="Q4" s="104"/>
-      <c r="R4" s="104"/>
-      <c r="S4" s="104"/>
-      <c r="T4" s="104"/>
-      <c r="U4" s="104"/>
-      <c r="V4" s="104"/>
-      <c r="W4" s="104"/>
-      <c r="X4" s="105"/>
+      <c r="O4" s="96"/>
+      <c r="P4" s="96"/>
+      <c r="Q4" s="96"/>
+      <c r="R4" s="96"/>
+      <c r="S4" s="96"/>
+      <c r="T4" s="96"/>
+      <c r="U4" s="96"/>
+      <c r="V4" s="96"/>
+      <c r="W4" s="96"/>
+      <c r="X4" s="97"/>
       <c r="Y4" s="27"/>
       <c r="Z4" s="27"/>
     </row>
     <row r="5" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="103"/>
-      <c r="B5" s="104"/>
-      <c r="C5" s="104"/>
-      <c r="D5" s="104"/>
-      <c r="E5" s="104"/>
-      <c r="F5" s="104"/>
-      <c r="G5" s="104"/>
-      <c r="H5" s="104"/>
-      <c r="I5" s="104"/>
-      <c r="J5" s="104"/>
-      <c r="K5" s="104"/>
-      <c r="L5" s="104"/>
-      <c r="M5" s="105"/>
-      <c r="N5" s="103"/>
-      <c r="O5" s="104"/>
-      <c r="P5" s="104"/>
-      <c r="Q5" s="104"/>
-      <c r="R5" s="104"/>
-      <c r="S5" s="104"/>
-      <c r="T5" s="104"/>
-      <c r="U5" s="104"/>
-      <c r="V5" s="104"/>
-      <c r="W5" s="104"/>
-      <c r="X5" s="105"/>
+      <c r="A5" s="98"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="96"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="96"/>
+      <c r="I5" s="96"/>
+      <c r="J5" s="96"/>
+      <c r="K5" s="96"/>
+      <c r="L5" s="96"/>
+      <c r="M5" s="97"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="96"/>
+      <c r="P5" s="96"/>
+      <c r="Q5" s="96"/>
+      <c r="R5" s="96"/>
+      <c r="S5" s="96"/>
+      <c r="T5" s="96"/>
+      <c r="U5" s="96"/>
+      <c r="V5" s="96"/>
+      <c r="W5" s="96"/>
+      <c r="X5" s="97"/>
       <c r="Y5" s="26"/>
       <c r="Z5" s="26"/>
     </row>
@@ -31877,41 +31877,41 @@
       <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="100" t="s">
+      <c r="A7" s="99" t="s">
         <v>91</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="100" t="s">
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="K7" s="39"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="39"/>
-      <c r="O7" s="39"/>
-      <c r="P7" s="100" t="s">
+      <c r="K7" s="45"/>
+      <c r="L7" s="45"/>
+      <c r="M7" s="45"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="45"/>
+      <c r="P7" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="Q7" s="39"/>
-      <c r="R7" s="39"/>
-      <c r="S7" s="39"/>
-      <c r="T7" s="39"/>
-      <c r="U7" s="39"/>
-      <c r="V7" s="39"/>
-      <c r="W7" s="39"/>
-      <c r="X7" s="39"/>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="45"/>
+      <c r="S7" s="45"/>
+      <c r="T7" s="45"/>
+      <c r="U7" s="45"/>
+      <c r="V7" s="45"/>
+      <c r="W7" s="45"/>
+      <c r="X7" s="45"/>
       <c r="Y7" s="27"/>
       <c r="Z7" s="27"/>
     </row>
     <row r="8" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="101"/>
+      <c r="A8" s="100"/>
       <c r="B8" s="31"/>
       <c r="C8" s="31"/>
       <c r="D8" s="31"/>
@@ -31920,7 +31920,7 @@
       <c r="G8" s="31"/>
       <c r="H8" s="31"/>
       <c r="I8" s="32"/>
-      <c r="J8" s="102" t="s">
+      <c r="J8" s="101" t="s">
         <v>92</v>
       </c>
       <c r="K8" s="31"/>
@@ -31928,7 +31928,7 @@
       <c r="M8" s="31"/>
       <c r="N8" s="31"/>
       <c r="O8" s="32"/>
-      <c r="P8" s="102" t="s">
+      <c r="P8" s="101" t="s">
         <v>93</v>
       </c>
       <c r="Q8" s="31"/>
@@ -31971,37 +31971,37 @@
       <c r="Z9" s="26"/>
     </row>
     <row r="10" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="64" t="s">
+      <c r="A10" s="89" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="42"/>
-      <c r="O10" s="42"/>
-      <c r="P10" s="42"/>
-      <c r="Q10" s="42"/>
-      <c r="R10" s="42"/>
-      <c r="S10" s="42"/>
-      <c r="T10" s="42"/>
-      <c r="U10" s="42"/>
-      <c r="V10" s="42"/>
-      <c r="W10" s="42"/>
-      <c r="X10" s="42"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="38"/>
+      <c r="R10" s="38"/>
+      <c r="S10" s="38"/>
+      <c r="T10" s="38"/>
+      <c r="U10" s="38"/>
+      <c r="V10" s="38"/>
+      <c r="W10" s="38"/>
+      <c r="X10" s="38"/>
       <c r="Y10" s="26"/>
       <c r="Z10" s="26"/>
     </row>
     <row r="11" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="89" t="s">
+      <c r="A11" s="58" t="s">
         <v>67</v>
       </c>
       <c r="B11" s="31"/>
@@ -32009,7 +32009,7 @@
       <c r="D11" s="31"/>
       <c r="E11" s="31"/>
       <c r="F11" s="32"/>
-      <c r="G11" s="89" t="s">
+      <c r="G11" s="58" t="s">
         <v>95</v>
       </c>
       <c r="H11" s="31"/>
@@ -32017,7 +32017,7 @@
       <c r="J11" s="31"/>
       <c r="K11" s="31"/>
       <c r="L11" s="32"/>
-      <c r="M11" s="89" t="s">
+      <c r="M11" s="58" t="s">
         <v>96</v>
       </c>
       <c r="N11" s="31"/>
@@ -32025,7 +32025,7 @@
       <c r="P11" s="31"/>
       <c r="Q11" s="31"/>
       <c r="R11" s="32"/>
-      <c r="S11" s="89" t="s">
+      <c r="S11" s="58" t="s">
         <v>97</v>
       </c>
       <c r="T11" s="31"/>
@@ -32065,41 +32065,41 @@
       <c r="Z12" s="26"/>
     </row>
     <row r="13" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="100" t="s">
+      <c r="A13" s="99" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="100" t="s">
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="K13" s="39"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="39"/>
-      <c r="O13" s="39"/>
-      <c r="P13" s="100" t="s">
+      <c r="K13" s="45"/>
+      <c r="L13" s="45"/>
+      <c r="M13" s="45"/>
+      <c r="N13" s="45"/>
+      <c r="O13" s="45"/>
+      <c r="P13" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="Q13" s="39"/>
-      <c r="R13" s="39"/>
-      <c r="S13" s="39"/>
-      <c r="T13" s="39"/>
-      <c r="U13" s="39"/>
-      <c r="V13" s="39"/>
-      <c r="W13" s="39"/>
-      <c r="X13" s="39"/>
+      <c r="Q13" s="45"/>
+      <c r="R13" s="45"/>
+      <c r="S13" s="45"/>
+      <c r="T13" s="45"/>
+      <c r="U13" s="45"/>
+      <c r="V13" s="45"/>
+      <c r="W13" s="45"/>
+      <c r="X13" s="45"/>
       <c r="Y13" s="27"/>
       <c r="Z13" s="27"/>
     </row>
     <row r="14" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="101"/>
+      <c r="A14" s="100"/>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
       <c r="D14" s="31"/>
@@ -32108,7 +32108,7 @@
       <c r="G14" s="31"/>
       <c r="H14" s="31"/>
       <c r="I14" s="32"/>
-      <c r="J14" s="102" t="s">
+      <c r="J14" s="101" t="s">
         <v>98</v>
       </c>
       <c r="K14" s="31"/>
@@ -32116,7 +32116,7 @@
       <c r="M14" s="31"/>
       <c r="N14" s="31"/>
       <c r="O14" s="32"/>
-      <c r="P14" s="102" t="s">
+      <c r="P14" s="101" t="s">
         <v>99</v>
       </c>
       <c r="Q14" s="31"/>
@@ -32159,102 +32159,102 @@
       <c r="Z15" s="26"/>
     </row>
     <row r="16" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="88" t="s">
+      <c r="A16" s="71" t="s">
         <v>100</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="52" t="s">
+      <c r="B16" s="45"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="K16" s="42"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="42"/>
-      <c r="N16" s="88" t="s">
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="O16" s="39"/>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="39"/>
-      <c r="R16" s="39"/>
-      <c r="S16" s="39"/>
-      <c r="T16" s="98" t="s">
+      <c r="O16" s="45"/>
+      <c r="P16" s="45"/>
+      <c r="Q16" s="45"/>
+      <c r="R16" s="45"/>
+      <c r="S16" s="45"/>
+      <c r="T16" s="107" t="s">
         <v>102</v>
       </c>
-      <c r="U16" s="39"/>
-      <c r="V16" s="39"/>
-      <c r="W16" s="39"/>
-      <c r="X16" s="39"/>
+      <c r="U16" s="45"/>
+      <c r="V16" s="45"/>
+      <c r="W16" s="45"/>
+      <c r="X16" s="45"/>
       <c r="Y16" s="13"/>
       <c r="Z16" s="13"/>
     </row>
     <row r="17" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="95" t="s">
+      <c r="A17" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="96" t="s">
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="105" t="s">
         <v>104</v>
       </c>
-      <c r="K17" s="36"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="37"/>
-      <c r="N17" s="95" t="s">
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="104" t="s">
         <v>105</v>
       </c>
-      <c r="O17" s="36"/>
-      <c r="P17" s="36"/>
-      <c r="Q17" s="36"/>
-      <c r="R17" s="36"/>
-      <c r="S17" s="37"/>
-      <c r="T17" s="95" t="s">
+      <c r="O17" s="35"/>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="35"/>
+      <c r="R17" s="35"/>
+      <c r="S17" s="36"/>
+      <c r="T17" s="104" t="s">
         <v>106</v>
       </c>
-      <c r="U17" s="36"/>
-      <c r="V17" s="36"/>
-      <c r="W17" s="36"/>
-      <c r="X17" s="37"/>
+      <c r="U17" s="35"/>
+      <c r="V17" s="35"/>
+      <c r="W17" s="35"/>
+      <c r="X17" s="36"/>
       <c r="Y17" s="26"/>
       <c r="Z17" s="26"/>
     </row>
     <row r="18" spans="1:26" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="42"/>
-      <c r="L18" s="42"/>
-      <c r="M18" s="43"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="42"/>
-      <c r="P18" s="42"/>
-      <c r="Q18" s="42"/>
-      <c r="R18" s="42"/>
-      <c r="S18" s="43"/>
-      <c r="T18" s="41"/>
-      <c r="U18" s="42"/>
-      <c r="V18" s="42"/>
-      <c r="W18" s="42"/>
-      <c r="X18" s="43"/>
+      <c r="A18" s="37"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="37"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="38"/>
+      <c r="R18" s="38"/>
+      <c r="S18" s="39"/>
+      <c r="T18" s="37"/>
+      <c r="U18" s="38"/>
+      <c r="V18" s="38"/>
+      <c r="W18" s="38"/>
+      <c r="X18" s="39"/>
       <c r="Y18" s="26"/>
       <c r="Z18" s="26"/>
     </row>
@@ -32315,36 +32315,36 @@
       <c r="Z20" s="26"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="97" t="s">
+      <c r="A21" s="106" t="s">
         <v>107</v>
       </c>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
       <c r="I21" s="28"/>
-      <c r="J21" s="97" t="s">
+      <c r="J21" s="106" t="s">
         <v>51</v>
       </c>
-      <c r="K21" s="36"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="36"/>
-      <c r="O21" s="36"/>
-      <c r="P21" s="36"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="35"/>
+      <c r="P21" s="35"/>
       <c r="Q21" s="29"/>
-      <c r="R21" s="97" t="s">
+      <c r="R21" s="106" t="s">
         <v>108</v>
       </c>
-      <c r="S21" s="36"/>
-      <c r="T21" s="36"/>
-      <c r="U21" s="36"/>
-      <c r="V21" s="36"/>
-      <c r="W21" s="36"/>
-      <c r="X21" s="36"/>
+      <c r="S21" s="35"/>
+      <c r="T21" s="35"/>
+      <c r="U21" s="35"/>
+      <c r="V21" s="35"/>
+      <c r="W21" s="35"/>
+      <c r="X21" s="35"/>
       <c r="Y21" s="26"/>
       <c r="Z21" s="26"/>
     </row>
@@ -32392,19 +32392,19 @@
       <c r="M23" s="26"/>
       <c r="N23" s="26"/>
       <c r="O23" s="26"/>
-      <c r="P23" s="93" t="s">
+      <c r="P23" s="102" t="s">
         <v>109</v>
       </c>
-      <c r="Q23" s="39"/>
-      <c r="R23" s="39"/>
-      <c r="S23" s="39"/>
-      <c r="T23" s="39"/>
-      <c r="U23" s="99" t="s">
+      <c r="Q23" s="45"/>
+      <c r="R23" s="45"/>
+      <c r="S23" s="45"/>
+      <c r="T23" s="45"/>
+      <c r="U23" s="108" t="s">
         <v>110</v>
       </c>
-      <c r="V23" s="42"/>
-      <c r="W23" s="42"/>
-      <c r="X23" s="42"/>
+      <c r="V23" s="38"/>
+      <c r="W23" s="38"/>
+      <c r="X23" s="38"/>
       <c r="Y23" s="26"/>
       <c r="Z23" s="26"/>
     </row>
@@ -32424,14 +32424,14 @@
       <c r="M24" s="26"/>
       <c r="N24" s="26"/>
       <c r="O24" s="26"/>
-      <c r="P24" s="93" t="s">
+      <c r="P24" s="102" t="s">
         <v>111</v>
       </c>
-      <c r="Q24" s="39"/>
-      <c r="R24" s="39"/>
-      <c r="S24" s="39"/>
-      <c r="T24" s="39"/>
-      <c r="U24" s="94" t="s">
+      <c r="Q24" s="45"/>
+      <c r="R24" s="45"/>
+      <c r="S24" s="45"/>
+      <c r="T24" s="45"/>
+      <c r="U24" s="103" t="s">
         <v>112</v>
       </c>
       <c r="V24" s="31"/>
@@ -59770,31 +59770,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="U2:X3"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
-    <mergeCell ref="J13:O13"/>
-    <mergeCell ref="P13:X13"/>
-    <mergeCell ref="A13:I13"/>
-    <mergeCell ref="A14:I14"/>
-    <mergeCell ref="J14:O14"/>
-    <mergeCell ref="P14:X14"/>
     <mergeCell ref="P24:T24"/>
     <mergeCell ref="U24:X24"/>
     <mergeCell ref="A16:I16"/>
@@ -59810,6 +59785,31 @@
     <mergeCell ref="R21:X21"/>
     <mergeCell ref="P23:T23"/>
     <mergeCell ref="U23:X23"/>
+    <mergeCell ref="J13:O13"/>
+    <mergeCell ref="P13:X13"/>
+    <mergeCell ref="A13:I13"/>
+    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="J14:O14"/>
+    <mergeCell ref="P14:X14"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0" footer="0"/>
   <pageSetup scale="95" orientation="landscape"/>

</xml_diff>